<commit_message>
confidence score + DataOnly
Fixed confidence score issue so that the values display correctly.
</commit_message>
<xml_diff>
--- a/Columns reference.xlsx
+++ b/Columns reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/ottwardu_uwaterloo_ca/Documents/Documents/GitHub/Forecasting-Tournament/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="14_{0086EA9A-E4BC-417D-A9D4-CBCF45C143D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8C6B225-3FC1-45E0-8B75-C2731D999A72}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="14_{0086EA9A-E4BC-417D-A9D4-CBCF45C143D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33C81935-E1F8-46D3-83E2-CD7DC8E5A92A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BFB2704-2340-4873-B614-2DBCF2A7F097}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="318">
   <si>
     <t>Column</t>
   </si>
@@ -991,6 +991,27 @@
   </si>
   <si>
     <t>the absolute percentage change between the team's prediction for that month and the matching ground truth data for that domain + month</t>
+  </si>
+  <si>
+    <t>DataOnly</t>
+  </si>
+  <si>
+    <t>0 = additional parameters / variables considered, 1 = only used data provided</t>
+  </si>
+  <si>
+    <t>Indicates whether participants relied solely on the data provided for the domain(s)</t>
+  </si>
+  <si>
+    <t>Coded by co-author (Oliver)</t>
+  </si>
+  <si>
+    <t>counterNum</t>
+  </si>
+  <si>
+    <t>Indicates the number of unique counterfactuals the participant considered</t>
+  </si>
+  <si>
+    <t>1-7 scale</t>
   </si>
 </sst>
 </file>
@@ -1377,10 +1398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEA65C1-8882-443D-817E-6C0B47AAF061}">
-  <dimension ref="A1:D190"/>
+  <dimension ref="A1:E192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="D180" sqref="D180"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1391,7 +1412,7 @@
     <col min="4" max="4" width="98.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>297</v>
       </c>
@@ -1405,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>93</v>
       </c>
@@ -1419,7 +1440,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>168</v>
       </c>
@@ -1433,7 +1454,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>101</v>
       </c>
@@ -1447,132 +1468,141 @@
         <v>305</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>120</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>243</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>51</v>
       </c>
-      <c r="C13" t="s">
-        <v>187</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C14" t="s">
+        <v>187</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>52</v>
       </c>
-      <c r="C14" t="s">
-        <v>187</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>111</v>
       </c>
-      <c r="C16" t="s">
-        <v>188</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>304</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" t="s">
-        <v>188</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>188</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" t="s">
-        <v>188</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>212</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>188</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>233</v>
@@ -1580,7 +1610,7 @@
     </row>
     <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>233</v>
@@ -1588,7 +1618,7 @@
     </row>
     <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>233</v>
@@ -1596,728 +1626,731 @@
     </row>
     <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" t="s">
-        <v>243</v>
+        <v>100</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>137</v>
       </c>
       <c r="C25" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C26" t="s">
         <v>266</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C27" t="s">
         <v>266</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>181</v>
       </c>
       <c r="C28" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>193</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>187</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>260</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>155</v>
+      </c>
+      <c r="B30" t="s">
+        <v>317</v>
+      </c>
+      <c r="C30" t="s">
+        <v>187</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" t="s">
-        <v>188</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>217</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
         <v>188</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
         <v>188</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>243</v>
+        <v>188</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>315</v>
       </c>
       <c r="C35" t="s">
         <v>188</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>242</v>
+        <v>316</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="C36" t="s">
-        <v>187</v>
+        <v>243</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="C37" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>290</v>
+        <v>187</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>290</v>
+        <v>187</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>287</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C40" t="s">
         <v>290</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C41" t="s">
         <v>290</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C42" t="s">
         <v>290</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C43" t="s">
         <v>290</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C44" t="s">
         <v>290</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C45" t="s">
         <v>290</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C46" t="s">
         <v>290</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C47" t="s">
         <v>290</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C48" t="s">
         <v>290</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C49" t="s">
         <v>290</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C50" t="s">
-        <v>187</v>
+        <v>290</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C51" t="s">
-        <v>187</v>
+        <v>290</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="C52" t="s">
         <v>187</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>223</v>
+        <v>292</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C53" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>215</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>146</v>
+        <v>88</v>
+      </c>
+      <c r="C54" t="s">
+        <v>187</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>165</v>
+        <v>78</v>
+      </c>
+      <c r="C55" t="s">
+        <v>188</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>29</v>
-      </c>
-      <c r="C57" t="s">
-        <v>187</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" t="s">
-        <v>187</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="C59" t="s">
-        <v>243</v>
+        <v>187</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>248</v>
+        <v>194</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
+        <v>187</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" t="s">
+        <v>243</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>5</v>
       </c>
-      <c r="C60" t="s">
-        <v>187</v>
-      </c>
-      <c r="D60" s="1" t="s">
+      <c r="C62" t="s">
+        <v>187</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="63" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="64" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>130</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C64" t="s">
         <v>243</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>26</v>
-      </c>
-      <c r="C64" t="s">
-        <v>188</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>163</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>261</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C66" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>163</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>164</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C68" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>126</v>
-      </c>
-      <c r="C69" t="s">
-        <v>243</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>246</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>127</v>
-      </c>
-      <c r="C70" t="s">
+        <v>164</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>126</v>
+      </c>
+      <c r="C71" t="s">
         <v>243</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>162</v>
+      <c r="D71" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>159</v>
+        <v>127</v>
+      </c>
+      <c r="C72" t="s">
+        <v>243</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>136</v>
-      </c>
-      <c r="C73" t="s">
-        <v>243</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>255</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>21</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="C75" t="s">
-        <v>187</v>
+        <v>243</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>222</v>
+        <v>255</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="C77" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>168</v>
+        <v>7</v>
       </c>
       <c r="C78" t="s">
         <v>187</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C79" t="s">
         <v>188</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>143</v>
+        <v>168</v>
+      </c>
+      <c r="C80" t="s">
+        <v>187</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>17</v>
+        <v>92</v>
+      </c>
+      <c r="C81" t="s">
+        <v>188</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>18</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>293</v>
-      </c>
-      <c r="C83" t="s">
-        <v>290</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>295</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>294</v>
-      </c>
-      <c r="C84" t="s">
-        <v>290</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>296</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>172</v>
+        <v>293</v>
       </c>
       <c r="C85" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>294</v>
       </c>
       <c r="C86" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>269</v>
+        <v>296</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C87" t="s">
         <v>266</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C88" t="s">
         <v>266</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C89" t="s">
         <v>266</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C90" t="s">
         <v>266</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="C91" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>107</v>
+        <v>173</v>
       </c>
       <c r="C92" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>239</v>
+        <v>268</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C93" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="C94" t="s">
         <v>187</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>207</v>
+        <v>239</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>31</v>
+        <v>108</v>
       </c>
       <c r="C95" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>197</v>
+        <v>240</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C96" t="s">
         <v>187</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C97" t="s">
         <v>187</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C98" t="s">
         <v>187</v>
@@ -2328,10 +2361,10 @@
     </row>
     <row r="99" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C99" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>203</v>
@@ -2339,10 +2372,10 @@
     </row>
     <row r="100" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C100" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>203</v>
@@ -2350,7 +2383,7 @@
     </row>
     <row r="101" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C101" t="s">
         <v>188</v>
@@ -2361,7 +2394,7 @@
     </row>
     <row r="102" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C102" t="s">
         <v>188</v>
@@ -2372,7 +2405,7 @@
     </row>
     <row r="103" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C103" t="s">
         <v>188</v>
@@ -2383,7 +2416,7 @@
     </row>
     <row r="104" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C104" t="s">
         <v>188</v>
@@ -2394,84 +2427,84 @@
     </row>
     <row r="105" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C105" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C106" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C107" t="s">
         <v>187</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C108" t="s">
         <v>187</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C109" t="s">
         <v>187</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C110" t="s">
         <v>187</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C111" t="s">
         <v>187</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C112" t="s">
         <v>187</v>
@@ -2482,435 +2515,441 @@
     </row>
     <row r="113" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>95</v>
+        <v>38</v>
+      </c>
+      <c r="C113" t="s">
+        <v>187</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C114" t="s">
         <v>187</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>129</v>
-      </c>
-      <c r="C115" t="s">
-        <v>243</v>
+        <v>95</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>161</v>
+        <v>56</v>
+      </c>
+      <c r="C116" t="s">
+        <v>187</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>158</v>
+        <v>129</v>
+      </c>
+      <c r="C117" t="s">
+        <v>243</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>84</v>
-      </c>
-      <c r="C120" t="s">
-        <v>188</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>221</v>
+        <v>167</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>89</v>
-      </c>
-      <c r="C121" t="s">
-        <v>187</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>223</v>
+        <v>166</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C122" t="s">
         <v>188</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C123" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>144</v>
+        <v>82</v>
+      </c>
+      <c r="C124" t="s">
+        <v>188</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C125" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>93</v>
-      </c>
-      <c r="C126" t="s">
-        <v>187</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>229</v>
+        <v>144</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>138</v>
+        <v>55</v>
       </c>
       <c r="C127" t="s">
-        <v>243</v>
+        <v>187</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>257</v>
+        <v>209</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="C128" t="s">
-        <v>243</v>
+        <v>187</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>183</v>
+        <v>138</v>
+      </c>
+      <c r="C129" t="s">
+        <v>243</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C130" t="s">
-        <v>187</v>
+        <v>243</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>109</v>
-      </c>
-      <c r="C131" t="s">
-        <v>188</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>241</v>
+        <v>183</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="C132" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>238</v>
+        <v>259</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="C133" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="C134" t="s">
         <v>188</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>205</v>
+        <v>238</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="C135" t="s">
-        <v>188</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>230</v>
+        <v>187</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>96</v>
+        <v>50</v>
+      </c>
+      <c r="C136" t="s">
+        <v>188</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>15</v>
+        <v>94</v>
+      </c>
+      <c r="C137" t="s">
+        <v>188</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>14</v>
+        <v>96</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>11</v>
-      </c>
-      <c r="C140" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>131</v>
-      </c>
-      <c r="C141" t="s">
-        <v>243</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>251</v>
+        <v>13</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>132</v>
+        <v>11</v>
       </c>
       <c r="C142" t="s">
-        <v>243</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C143" t="s">
         <v>243</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>12</v>
+        <v>132</v>
       </c>
       <c r="C144" t="s">
-        <v>187</v>
+        <v>243</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="C145" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>177</v>
+        <v>12</v>
       </c>
       <c r="C146" t="s">
-        <v>266</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>272</v>
+        <v>187</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>178</v>
+        <v>101</v>
       </c>
       <c r="C147" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>273</v>
+        <v>232</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C148" t="s">
         <v>266</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>140</v>
+        <v>178</v>
       </c>
       <c r="C149" t="s">
-        <v>243</v>
+        <v>266</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="C150" t="s">
-        <v>243</v>
+        <v>266</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="C151" t="s">
-        <v>187</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="C152" t="s">
-        <v>188</v>
+        <v>243</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>4</v>
-      </c>
-      <c r="B153" t="s">
-        <v>196</v>
+        <v>87</v>
       </c>
       <c r="C153" t="s">
         <v>187</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>184</v>
+        <v>224</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="C154" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>139</v>
+        <v>4</v>
+      </c>
+      <c r="B155" t="s">
+        <v>196</v>
       </c>
       <c r="C155" t="s">
-        <v>243</v>
+        <v>187</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>258</v>
+        <v>184</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="C156" t="s">
-        <v>188</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="C157" t="s">
         <v>243</v>
       </c>
+      <c r="D157" s="1" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="158" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="C158" t="s">
-        <v>243</v>
+        <v>188</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C159" t="s">
         <v>243</v>
@@ -2918,7 +2957,7 @@
     </row>
     <row r="160" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C160" t="s">
         <v>243</v>
@@ -2926,7 +2965,7 @@
     </row>
     <row r="161" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C161" t="s">
         <v>243</v>
@@ -2934,7 +2973,7 @@
     </row>
     <row r="162" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C162" t="s">
         <v>243</v>
@@ -2942,7 +2981,7 @@
     </row>
     <row r="163" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C163" t="s">
         <v>243</v>
@@ -2950,7 +2989,7 @@
     </row>
     <row r="164" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C164" t="s">
         <v>243</v>
@@ -2958,7 +2997,7 @@
     </row>
     <row r="165" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C165" t="s">
         <v>243</v>
@@ -2966,7 +3005,7 @@
     </row>
     <row r="166" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C166" t="s">
         <v>243</v>
@@ -2974,7 +3013,7 @@
     </row>
     <row r="167" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C167" t="s">
         <v>243</v>
@@ -2982,7 +3021,7 @@
     </row>
     <row r="168" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C168" t="s">
         <v>243</v>
@@ -2990,198 +3029,214 @@
     </row>
     <row r="169" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="C169" t="s">
-        <v>188</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>189</v>
+        <v>243</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C170" t="s">
-        <v>188</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C171" t="s">
         <v>188</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C172" t="s">
         <v>188</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>104</v>
+        <v>23</v>
       </c>
       <c r="C173" t="s">
         <v>188</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="C174" t="s">
         <v>188</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>190</v>
+        <v>234</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="C175" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>208</v>
+        <v>236</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C176" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>223</v>
+        <v>190</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>182</v>
+        <v>54</v>
+      </c>
+      <c r="C177" t="s">
+        <v>187</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>169</v>
+        <v>86</v>
+      </c>
+      <c r="C178" t="s">
+        <v>187</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>74</v>
-      </c>
-      <c r="C183" t="s">
-        <v>188</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>213</v>
+        <v>148</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>75</v>
-      </c>
-      <c r="C184" t="s">
-        <v>188</v>
-      </c>
-      <c r="D184" s="1" t="s">
-        <v>214</v>
+        <v>149</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="C185" t="s">
+        <v>188</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="C186" t="s">
+        <v>188</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>30</v>
-      </c>
-      <c r="C187" t="s">
-        <v>187</v>
-      </c>
-      <c r="D187" s="1" t="s">
-        <v>195</v>
+        <v>76</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>30</v>
+      </c>
+      <c r="C189" t="s">
+        <v>187</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>306</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B191" t="s">
         <v>307</v>
       </c>
-      <c r="C189" t="s">
-        <v>187</v>
-      </c>
-      <c r="D189" s="1" t="s">
+      <c r="C191" t="s">
+        <v>187</v>
+      </c>
+      <c r="D191" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+    <row r="192" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>309</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B192" t="s">
         <v>307</v>
       </c>
-      <c r="C190" t="s">
-        <v>187</v>
-      </c>
-      <c r="D190" s="1" t="s">
+      <c r="C192" t="s">
+        <v>187</v>
+      </c>
+      <c r="D192" s="1" t="s">
         <v>310</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:D188">
-    <sortCondition ref="A7:A188"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D190">
+    <sortCondition ref="A8:A190"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
removed NAs from columns
removed NAs from team size and numpred columns
</commit_message>
<xml_diff>
--- a/Columns reference.xlsx
+++ b/Columns reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/ottwardu_uwaterloo_ca/Documents/Documents/GitHub/Forecasting-Tournament/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="14_{0086EA9A-E4BC-417D-A9D4-CBCF45C143D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33C81935-E1F8-46D3-83E2-CD7DC8E5A92A}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="14_{0086EA9A-E4BC-417D-A9D4-CBCF45C143D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C173F18-5063-4AD6-884D-091D2AE16DBE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BFB2704-2340-4873-B614-2DBCF2A7F097}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -361,9 +362,6 @@
   </si>
   <si>
     <t>Method.complex</t>
-  </si>
-  <si>
-    <t>Presence.Final</t>
   </si>
   <si>
     <t>COVID.Final</t>
@@ -1012,6 +1010,9 @@
   </si>
   <si>
     <t>1-7 scale</t>
+  </si>
+  <si>
+    <t>CounterFactual_Presence.Final</t>
   </si>
 </sst>
 </file>
@@ -1401,7 +1402,7 @@
   <dimension ref="A1:E192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,10 +1415,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>297</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>298</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -1431,27 +1432,27 @@
         <v>93</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1459,30 +1460,30 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="C5" t="s">
-        <v>188</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1501,38 +1502,38 @@
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1540,10 +1541,10 @@
         <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1551,26 +1552,26 @@
         <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1578,15 +1579,15 @@
         <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1594,10 +1595,10 @@
         <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1605,7 +1606,7 @@
         <v>97</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1613,7 +1614,7 @@
         <v>98</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1621,7 +1622,7 @@
         <v>99</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1629,51 +1630,51 @@
         <v>100</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C27" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C28" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1681,24 +1682,24 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1711,10 +1712,10 @@
         <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1722,10 +1723,10 @@
         <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1733,43 +1734,43 @@
         <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>314</v>
+      </c>
+      <c r="C35" t="s">
+        <v>187</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="C35" t="s">
-        <v>188</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C36" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1777,10 +1778,10 @@
         <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1788,10 +1789,10 @@
         <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1799,10 +1800,10 @@
         <v>61</v>
       </c>
       <c r="C40" t="s">
+        <v>289</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1810,10 +1811,10 @@
         <v>70</v>
       </c>
       <c r="C41" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1821,10 +1822,10 @@
         <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1832,10 +1833,10 @@
         <v>72</v>
       </c>
       <c r="C43" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1843,10 +1844,10 @@
         <v>62</v>
       </c>
       <c r="C44" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1854,10 +1855,10 @@
         <v>63</v>
       </c>
       <c r="C45" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1865,10 +1866,10 @@
         <v>64</v>
       </c>
       <c r="C46" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1876,10 +1877,10 @@
         <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1887,10 +1888,10 @@
         <v>66</v>
       </c>
       <c r="C48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1898,10 +1899,10 @@
         <v>67</v>
       </c>
       <c r="C49" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1909,10 +1910,10 @@
         <v>68</v>
       </c>
       <c r="C50" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1920,10 +1921,10 @@
         <v>69</v>
       </c>
       <c r="C51" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1931,10 +1932,10 @@
         <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1942,10 +1943,10 @@
         <v>59</v>
       </c>
       <c r="C53" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1953,10 +1954,10 @@
         <v>88</v>
       </c>
       <c r="C54" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1964,20 +1965,20 @@
         <v>78</v>
       </c>
       <c r="C55" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1990,10 +1991,10 @@
         <v>29</v>
       </c>
       <c r="C59" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2001,21 +2002,21 @@
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C61" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2023,26 +2024,26 @@
         <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C64" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2055,18 +2056,18 @@
         <v>26</v>
       </c>
       <c r="C66" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2074,63 +2075,63 @@
         <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C71" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C72" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C75" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2143,10 +2144,10 @@
         <v>85</v>
       </c>
       <c r="C77" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2154,7 +2155,7 @@
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2162,21 +2163,21 @@
         <v>105</v>
       </c>
       <c r="C79" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C80" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2184,15 +2185,15 @@
         <v>92</v>
       </c>
       <c r="C81" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2207,90 +2208,90 @@
     </row>
     <row r="85" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C85" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C86" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C87" t="s">
+        <v>265</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C88" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C89" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C90" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C91" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C92" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2298,10 +2299,10 @@
         <v>90</v>
       </c>
       <c r="C93" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2309,10 +2310,10 @@
         <v>107</v>
       </c>
       <c r="C94" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2320,10 +2321,10 @@
         <v>108</v>
       </c>
       <c r="C95" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2331,10 +2332,10 @@
         <v>53</v>
       </c>
       <c r="C96" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2342,10 +2343,10 @@
         <v>31</v>
       </c>
       <c r="C97" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2353,10 +2354,10 @@
         <v>40</v>
       </c>
       <c r="C98" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2364,10 +2365,10 @@
         <v>41</v>
       </c>
       <c r="C99" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2375,10 +2376,10 @@
         <v>42</v>
       </c>
       <c r="C100" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2386,10 +2387,10 @@
         <v>43</v>
       </c>
       <c r="C101" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2397,10 +2398,10 @@
         <v>44</v>
       </c>
       <c r="C102" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2408,10 +2409,10 @@
         <v>45</v>
       </c>
       <c r="C103" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2419,10 +2420,10 @@
         <v>46</v>
       </c>
       <c r="C104" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2430,10 +2431,10 @@
         <v>47</v>
       </c>
       <c r="C105" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2441,10 +2442,10 @@
         <v>48</v>
       </c>
       <c r="C106" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2452,10 +2453,10 @@
         <v>32</v>
       </c>
       <c r="C107" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2463,10 +2464,10 @@
         <v>33</v>
       </c>
       <c r="C108" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2474,10 +2475,10 @@
         <v>34</v>
       </c>
       <c r="C109" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2485,10 +2486,10 @@
         <v>35</v>
       </c>
       <c r="C110" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2496,10 +2497,10 @@
         <v>36</v>
       </c>
       <c r="C111" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2507,10 +2508,10 @@
         <v>37</v>
       </c>
       <c r="C112" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2518,10 +2519,10 @@
         <v>38</v>
       </c>
       <c r="C113" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2529,10 +2530,10 @@
         <v>39</v>
       </c>
       <c r="C114" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2540,7 +2541,7 @@
         <v>95</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2548,41 +2549,41 @@
         <v>56</v>
       </c>
       <c r="C116" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C117" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2590,10 +2591,10 @@
         <v>84</v>
       </c>
       <c r="C122" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2601,10 +2602,10 @@
         <v>89</v>
       </c>
       <c r="C123" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2612,10 +2613,10 @@
         <v>82</v>
       </c>
       <c r="C124" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2623,15 +2624,15 @@
         <v>83</v>
       </c>
       <c r="C125" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2639,10 +2640,10 @@
         <v>55</v>
       </c>
       <c r="C127" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2650,59 +2651,59 @@
         <v>93</v>
       </c>
       <c r="C128" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C129" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C130" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C132" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>109</v>
+        <v>317</v>
       </c>
       <c r="C133" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2710,10 +2711,10 @@
         <v>106</v>
       </c>
       <c r="C134" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2721,7 +2722,7 @@
         <v>8</v>
       </c>
       <c r="C135" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2729,10 +2730,10 @@
         <v>50</v>
       </c>
       <c r="C136" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2740,10 +2741,10 @@
         <v>94</v>
       </c>
       <c r="C137" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2751,7 +2752,7 @@
         <v>96</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2774,40 +2775,40 @@
         <v>11</v>
       </c>
       <c r="C142" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C143" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C144" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C145" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2815,7 +2816,7 @@
         <v>12</v>
       </c>
       <c r="C146" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2823,62 +2824,62 @@
         <v>101</v>
       </c>
       <c r="C147" t="s">
+        <v>230</v>
+      </c>
+      <c r="D147" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C148" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C149" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C150" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C151" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C152" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2886,10 +2887,10 @@
         <v>87</v>
       </c>
       <c r="C153" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2897,10 +2898,10 @@
         <v>91</v>
       </c>
       <c r="C154" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2908,13 +2909,13 @@
         <v>4</v>
       </c>
       <c r="B155" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C155" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2922,18 +2923,18 @@
         <v>6</v>
       </c>
       <c r="C156" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C157" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2941,106 +2942,106 @@
         <v>49</v>
       </c>
       <c r="C158" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C159" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C160" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C161" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C162" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C163" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C164" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C165" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C166" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C167" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C168" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C169" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C170" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3048,10 +3049,10 @@
         <v>24</v>
       </c>
       <c r="C171" t="s">
+        <v>187</v>
+      </c>
+      <c r="D171" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3059,10 +3060,10 @@
         <v>103</v>
       </c>
       <c r="C172" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3070,7 +3071,7 @@
         <v>23</v>
       </c>
       <c r="C173" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3078,10 +3079,10 @@
         <v>102</v>
       </c>
       <c r="C174" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3089,10 +3090,10 @@
         <v>104</v>
       </c>
       <c r="C175" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3100,10 +3101,10 @@
         <v>25</v>
       </c>
       <c r="C176" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3111,10 +3112,10 @@
         <v>54</v>
       </c>
       <c r="C177" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3122,40 +3123,40 @@
         <v>86</v>
       </c>
       <c r="C178" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3163,10 +3164,10 @@
         <v>74</v>
       </c>
       <c r="C185" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3174,10 +3175,10 @@
         <v>75</v>
       </c>
       <c r="C186" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3195,10 +3196,10 @@
         <v>30</v>
       </c>
       <c r="C189" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3208,30 +3209,30 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>305</v>
+      </c>
+      <c r="B191" t="s">
         <v>306</v>
       </c>
-      <c r="B191" t="s">
+      <c r="C191" t="s">
+        <v>186</v>
+      </c>
+      <c r="D191" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="C191" t="s">
-        <v>187</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
+        <v>308</v>
+      </c>
+      <c r="B192" t="s">
+        <v>306</v>
+      </c>
+      <c r="C192" t="s">
+        <v>186</v>
+      </c>
+      <c r="D192" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="B192" t="s">
-        <v>307</v>
-      </c>
-      <c r="C192" t="s">
-        <v>187</v>
-      </c>
-      <c r="D192" s="1" t="s">
-        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prolific + team size updates
Updated team size, prolific methods + complexity, and added dataOnly column
</commit_message>
<xml_diff>
--- a/Columns reference.xlsx
+++ b/Columns reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/ottwardu_uwaterloo_ca/Documents/Documents/GitHub/Forecasting-Tournament/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="14_{0086EA9A-E4BC-417D-A9D4-CBCF45C143D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{394B799A-5019-42EE-9CFB-088562E5FD3C}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="14_{0086EA9A-E4BC-417D-A9D4-CBCF45C143D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D24D499-0C9F-4F3D-9882-64E679D9B042}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BFB2704-2340-4873-B614-2DBCF2A7F097}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="233">
   <si>
     <t>Description</t>
   </si>
@@ -773,6 +773,16 @@
   </si>
   <si>
     <t>Factor equivalent of RMSE_cutoff_Naive_rwf_w2</t>
+  </si>
+  <si>
+    <t>DataOnly</t>
+  </si>
+  <si>
+    <t>0 = other parameters considered
+1 = only used data provided</t>
+  </si>
+  <si>
+    <t>Only applies to rows that were coded as Data-Driven (3 for Method.coded). Indicates whether participant considered only data we provided or included additional parameters</t>
   </si>
 </sst>
 </file>
@@ -1147,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEA65C1-8882-443D-817E-6C0B47AAF061}">
-  <dimension ref="A1:E190"/>
+  <dimension ref="A1:E191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,24 +2034,24 @@
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>230</v>
+      </c>
+      <c r="B58" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" t="s">
+        <v>75</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E58" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>96</v>
-      </c>
-      <c r="B58" t="s">
-        <v>76</v>
-      </c>
-      <c r="C58" t="s">
-        <v>75</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E58" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>56</v>
       </c>
       <c r="B59" t="s">
         <v>76</v>
@@ -2050,29 +2060,32 @@
         <v>75</v>
       </c>
       <c r="D59" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E59" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60" t="s">
+        <v>76</v>
+      </c>
+      <c r="C60" t="s">
+        <v>75</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E60" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>57</v>
-      </c>
-      <c r="B60" t="s">
-        <v>77</v>
-      </c>
-      <c r="C60" t="s">
-        <v>104</v>
-      </c>
-      <c r="E60" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>58</v>
       </c>
       <c r="B61" t="s">
         <v>77</v>
@@ -2080,16 +2093,13 @@
       <c r="C61" t="s">
         <v>104</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="E61" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
         <v>77</v>
@@ -2098,15 +2108,15 @@
         <v>104</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E62" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B63" t="s">
         <v>77</v>
@@ -2115,15 +2125,15 @@
         <v>104</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="E63" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B64" t="s">
         <v>77</v>
@@ -2131,16 +2141,16 @@
       <c r="C64" t="s">
         <v>104</v>
       </c>
-      <c r="D64" t="s">
-        <v>163</v>
+      <c r="D64" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B65" t="s">
         <v>77</v>
@@ -2148,16 +2158,16 @@
       <c r="C65" t="s">
         <v>104</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E65" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>163</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B66" t="s">
         <v>77</v>
@@ -2166,15 +2176,15 @@
         <v>104</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="E66" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B67" t="s">
         <v>77</v>
@@ -2183,15 +2193,15 @@
         <v>104</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E67" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B68" t="s">
         <v>77</v>
@@ -2199,13 +2209,16 @@
       <c r="C68" t="s">
         <v>104</v>
       </c>
+      <c r="D68" s="1" t="s">
+        <v>168</v>
+      </c>
       <c r="E68" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B69" t="s">
         <v>77</v>
@@ -2213,16 +2226,13 @@
       <c r="C69" t="s">
         <v>104</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="E69" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B70" t="s">
         <v>77</v>
@@ -2231,29 +2241,32 @@
         <v>104</v>
       </c>
       <c r="D70" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E70" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>67</v>
+      </c>
+      <c r="B71" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71" t="s">
+        <v>104</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E71" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>174</v>
-      </c>
-      <c r="B71" t="s">
-        <v>75</v>
-      </c>
-      <c r="C71" t="s">
-        <v>104</v>
-      </c>
-      <c r="E71" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B72" t="s">
         <v>75</v>
@@ -2262,12 +2275,12 @@
         <v>104</v>
       </c>
       <c r="E72" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B73" t="s">
         <v>75</v>
@@ -2276,12 +2289,12 @@
         <v>104</v>
       </c>
       <c r="E73" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B74" t="s">
         <v>75</v>
@@ -2290,12 +2303,12 @@
         <v>104</v>
       </c>
       <c r="E74" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B75" t="s">
         <v>75</v>
@@ -2304,43 +2317,40 @@
         <v>104</v>
       </c>
       <c r="E75" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>182</v>
+      </c>
+      <c r="B76" t="s">
+        <v>75</v>
+      </c>
+      <c r="C76" t="s">
+        <v>104</v>
+      </c>
+      <c r="E76" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>183</v>
       </c>
-      <c r="B76" t="s">
-        <v>75</v>
-      </c>
-      <c r="C76" t="s">
-        <v>104</v>
-      </c>
-      <c r="E76" t="s">
+      <c r="B77" t="s">
+        <v>75</v>
+      </c>
+      <c r="C77" t="s">
+        <v>104</v>
+      </c>
+      <c r="E77" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>70</v>
-      </c>
-      <c r="B77" t="s">
-        <v>75</v>
-      </c>
-      <c r="C77" t="s">
-        <v>104</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E77" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B78" t="s">
         <v>75</v>
@@ -2352,29 +2362,29 @@
         <v>185</v>
       </c>
       <c r="E78" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>71</v>
+      </c>
+      <c r="B79" t="s">
+        <v>75</v>
+      </c>
+      <c r="C79" t="s">
+        <v>104</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E79" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>72</v>
-      </c>
-      <c r="B79" t="s">
-        <v>75</v>
-      </c>
-      <c r="C79" t="s">
-        <v>104</v>
-      </c>
-      <c r="D79" t="s">
-        <v>188</v>
-      </c>
-      <c r="E79" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B80" t="s">
         <v>75</v>
@@ -2383,15 +2393,15 @@
         <v>104</v>
       </c>
       <c r="D80" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E80" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>192</v>
+        <v>73</v>
       </c>
       <c r="B81" t="s">
         <v>75</v>
@@ -2399,13 +2409,16 @@
       <c r="C81" t="s">
         <v>104</v>
       </c>
+      <c r="D81" t="s">
+        <v>190</v>
+      </c>
       <c r="E81" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B82" t="s">
         <v>75</v>
@@ -2414,12 +2427,12 @@
         <v>104</v>
       </c>
       <c r="E82" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B83" t="s">
         <v>75</v>
@@ -2428,12 +2441,12 @@
         <v>104</v>
       </c>
       <c r="E83" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B84" t="s">
         <v>75</v>
@@ -2442,12 +2455,12 @@
         <v>104</v>
       </c>
       <c r="E84" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B85" t="s">
         <v>75</v>
@@ -2456,12 +2469,12 @@
         <v>104</v>
       </c>
       <c r="E85" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>200</v>
       </c>
       <c r="B86" t="s">
         <v>75</v>
@@ -2470,12 +2483,12 @@
         <v>104</v>
       </c>
       <c r="E86" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>202</v>
+        <v>93</v>
       </c>
       <c r="B87" t="s">
         <v>75</v>
@@ -2484,12 +2497,12 @@
         <v>104</v>
       </c>
       <c r="E87" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B88" t="s">
         <v>75</v>
@@ -2498,12 +2511,12 @@
         <v>104</v>
       </c>
       <c r="E88" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B89" t="s">
         <v>75</v>
@@ -2512,12 +2525,12 @@
         <v>104</v>
       </c>
       <c r="E89" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B90" t="s">
         <v>75</v>
@@ -2526,12 +2539,12 @@
         <v>104</v>
       </c>
       <c r="E90" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B91" t="s">
         <v>75</v>
@@ -2540,12 +2553,12 @@
         <v>104</v>
       </c>
       <c r="E91" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B92" t="s">
         <v>75</v>
@@ -2554,26 +2567,26 @@
         <v>104</v>
       </c>
       <c r="E92" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B93" t="s">
         <v>75</v>
       </c>
       <c r="C93" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E93" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B94" t="s">
         <v>75</v>
@@ -2582,12 +2595,12 @@
         <v>118</v>
       </c>
       <c r="E94" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B95" t="s">
         <v>75</v>
@@ -2596,12 +2609,12 @@
         <v>118</v>
       </c>
       <c r="E95" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B96" t="s">
         <v>75</v>
@@ -2610,12 +2623,12 @@
         <v>118</v>
       </c>
       <c r="E96" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B97" t="s">
         <v>75</v>
@@ -2623,14 +2636,13 @@
       <c r="C97" t="s">
         <v>118</v>
       </c>
-      <c r="D97" s="1"/>
       <c r="E97" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B98" t="s">
         <v>75</v>
@@ -2640,12 +2652,12 @@
       </c>
       <c r="D98" s="1"/>
       <c r="E98" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B99" t="s">
         <v>75</v>
@@ -2653,16 +2665,14 @@
       <c r="C99" t="s">
         <v>118</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>185</v>
-      </c>
+      <c r="D99" s="1"/>
       <c r="E99" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B100" t="s">
         <v>75</v>
@@ -2674,12 +2684,12 @@
         <v>185</v>
       </c>
       <c r="E100" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B101" t="s">
         <v>75</v>
@@ -2687,16 +2697,16 @@
       <c r="C101" t="s">
         <v>118</v>
       </c>
-      <c r="D101" t="s">
-        <v>188</v>
+      <c r="D101" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="E101" t="s">
-        <v>227</v>
+        <v>187</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B102" t="s">
         <v>75</v>
@@ -2705,13 +2715,29 @@
         <v>118</v>
       </c>
       <c r="D102" t="s">
+        <v>188</v>
+      </c>
+      <c r="E102" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>228</v>
+      </c>
+      <c r="B103" t="s">
+        <v>75</v>
+      </c>
+      <c r="C103" t="s">
+        <v>118</v>
+      </c>
+      <c r="D103" t="s">
         <v>190</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E103" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="145" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="146" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="147" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="148" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2757,10 +2783,12 @@
     <row r="188" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="189" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="190" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D190">
-    <sortCondition ref="A8:A190"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D191">
+    <sortCondition ref="A8:A191"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new variables for when teams submitted forecasts
</commit_message>
<xml_diff>
--- a/Columns reference.xlsx
+++ b/Columns reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igrossma\Documents\GitHub\Forecasting-Tournament\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/ottwardu_uwaterloo_ca/Documents/Documents/GitHub/Forecasting-Tournament/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9CA9E6-EFA6-4D9B-8143-CA724CACC61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9F9CA9E6-EFA6-4D9B-8143-CA724CACC61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A30F568-5DA6-4AE4-8D23-FC10E55A201F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3BFB2704-2340-4873-B614-2DBCF2A7F097}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BFB2704-2340-4873-B614-2DBCF2A7F097}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="241">
   <si>
     <t>Description</t>
   </si>
@@ -786,6 +786,27 @@
   </si>
   <si>
     <t>0 = Only submitted in one phase (initial forecasts for phase 1 / initial forecasts for phase 2), 1 = prediction in both phase 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>TournamentStart</t>
+  </si>
+  <si>
+    <t>"May", "October"</t>
+  </si>
+  <si>
+    <t>Indicates whether the team started in May or October</t>
+  </si>
+  <si>
+    <t>ForecastisUpdate</t>
+  </si>
+  <si>
+    <t>Phase 2</t>
+  </si>
+  <si>
+    <t>0 = no update, 1 = update</t>
+  </si>
+  <si>
+    <t>Indicates whether the team's forecast for phase 2 is an update of their previous forecast (1) or a new forecast (0)</t>
   </si>
 </sst>
 </file>
@@ -1162,19 +1183,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEA65C1-8882-443D-817E-6C0B47AAF061}">
   <dimension ref="A1:E191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.26953125" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" customWidth="1"/>
-    <col min="4" max="4" width="45.81640625" customWidth="1"/>
-    <col min="5" max="5" width="56.7265625" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
+    <col min="5" max="5" width="56.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>97</v>
       </c>
@@ -1191,7 +1212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1208,7 +1229,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1222,7 +1243,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1239,7 +1260,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="192" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="192" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1256,7 +1277,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1294,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1290,7 +1311,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1307,7 +1328,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1324,7 +1345,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1341,7 +1362,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1358,7 +1379,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1375,7 +1396,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1392,7 +1413,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1409,7 +1430,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1426,7 +1447,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1443,7 +1464,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1460,7 +1481,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1477,7 +1498,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1494,7 +1515,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1511,7 +1532,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1528,7 +1549,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1545,7 +1566,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1562,7 +1583,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1579,7 +1600,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1596,7 +1617,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1613,7 +1634,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1627,7 +1648,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1644,7 +1665,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1661,7 +1682,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1675,7 +1696,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1689,7 +1710,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1703,7 +1724,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1717,7 +1738,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1731,7 +1752,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1745,7 +1766,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1759,7 +1780,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1773,7 +1794,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1787,7 +1808,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1801,7 +1822,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1815,7 +1836,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1829,7 +1850,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1846,32 +1867,32 @@
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1888,7 +1909,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1905,7 +1926,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>69</v>
       </c>
@@ -1922,7 +1943,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1939,7 +1960,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1953,7 +1974,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1967,7 +1988,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1984,7 +2005,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2001,7 +2022,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2018,7 +2039,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2035,7 +2056,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>229</v>
       </c>
@@ -2052,7 +2073,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>96</v>
       </c>
@@ -2069,7 +2090,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>56</v>
       </c>
@@ -2086,7 +2107,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>57</v>
       </c>
@@ -2100,7 +2121,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -2117,7 +2138,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -2134,7 +2155,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>60</v>
       </c>
@@ -2151,7 +2172,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>61</v>
       </c>
@@ -2168,7 +2189,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>62</v>
       </c>
@@ -2185,7 +2206,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -2202,7 +2223,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>64</v>
       </c>
@@ -2219,7 +2240,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>65</v>
       </c>
@@ -2233,7 +2254,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>66</v>
       </c>
@@ -2250,7 +2271,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>67</v>
       </c>
@@ -2267,7 +2288,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>173</v>
       </c>
@@ -2281,7 +2302,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>175</v>
       </c>
@@ -2295,7 +2316,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>177</v>
       </c>
@@ -2309,7 +2330,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>179</v>
       </c>
@@ -2323,7 +2344,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>181</v>
       </c>
@@ -2337,7 +2358,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>182</v>
       </c>
@@ -2351,7 +2372,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>70</v>
       </c>
@@ -2368,7 +2389,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>71</v>
       </c>
@@ -2385,7 +2406,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>72</v>
       </c>
@@ -2402,7 +2423,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>73</v>
       </c>
@@ -2419,7 +2440,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>191</v>
       </c>
@@ -2433,7 +2454,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>193</v>
       </c>
@@ -2447,7 +2468,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>195</v>
       </c>
@@ -2461,7 +2482,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>197</v>
       </c>
@@ -2475,7 +2496,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>199</v>
       </c>
@@ -2489,7 +2510,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -2503,7 +2524,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>201</v>
       </c>
@@ -2517,7 +2538,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>203</v>
       </c>
@@ -2531,7 +2552,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>205</v>
       </c>
@@ -2545,7 +2566,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>207</v>
       </c>
@@ -2559,7 +2580,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>209</v>
       </c>
@@ -2573,7 +2594,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>210</v>
       </c>
@@ -2587,7 +2608,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>212</v>
       </c>
@@ -2601,7 +2622,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>214</v>
       </c>
@@ -2615,7 +2636,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>216</v>
       </c>
@@ -2629,7 +2650,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>218</v>
       </c>
@@ -2643,7 +2664,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>220</v>
       </c>
@@ -2658,7 +2679,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>221</v>
       </c>
@@ -2673,7 +2694,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>223</v>
       </c>
@@ -2690,7 +2711,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>224</v>
       </c>
@@ -2707,7 +2728,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>225</v>
       </c>
@@ -2724,7 +2745,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>227</v>
       </c>
@@ -2741,52 +2762,86 @@
         <v>228</v>
       </c>
     </row>
-    <row r="146" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="147" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="148" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="149" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="150" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="151" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="152" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="153" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="154" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="155" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="156" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="157" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="158" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="159" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="160" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="161" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="162" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="163" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="164" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="165" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="166" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="167" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="168" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="169" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="170" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="171" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="172" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="173" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="174" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="175" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="176" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="177" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="178" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="179" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="180" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="181" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="182" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="183" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="184" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="185" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="186" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="187" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="188" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="189" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="190" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="191" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>234</v>
+      </c>
+      <c r="B104" t="s">
+        <v>75</v>
+      </c>
+      <c r="C104" t="s">
+        <v>75</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E104" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>237</v>
+      </c>
+      <c r="B105" t="s">
+        <v>76</v>
+      </c>
+      <c r="C105" t="s">
+        <v>238</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E105" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="146" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D191">
     <sortCondition ref="A8:A191"/>

</xml_diff>

<commit_message>
Added columns for counterfactuals and revision rationale
</commit_message>
<xml_diff>
--- a/Columns reference.xlsx
+++ b/Columns reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/ottwardu_uwaterloo_ca/Documents/Documents/GitHub/Forecasting-Tournament/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{9F9CA9E6-EFA6-4D9B-8143-CA724CACC61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B2CCEEC-922E-44F2-80F6-BFDDEF07E98B}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="13_ncr:1_{9F9CA9E6-EFA6-4D9B-8143-CA724CACC61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28BC619A-DF51-4206-A653-64BA1F905946}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BFB2704-2340-4873-B614-2DBCF2A7F097}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="284">
   <si>
     <t>Description</t>
   </si>
@@ -782,9 +782,6 @@
     <t>Indicates whether the team started in May or October</t>
   </si>
   <si>
-    <t>ForecastisUpdate</t>
-  </si>
-  <si>
     <t>Phase 2</t>
   </si>
   <si>
@@ -873,13 +870,79 @@
   </si>
   <si>
     <t>Indicates whether one or more team members have participated in a forecasting tournament. Unlike previous_tournament.coded, teams that were missing team member responses were marked as NA</t>
+  </si>
+  <si>
+    <t>team_gender</t>
+  </si>
+  <si>
+    <t>team_education</t>
+  </si>
+  <si>
+    <t>team_Age</t>
+  </si>
+  <si>
+    <t>non_US</t>
+  </si>
+  <si>
+    <t>Onus.Final</t>
+  </si>
+  <si>
+    <t>counterNum</t>
+  </si>
+  <si>
+    <t>dataReceived_Final</t>
+  </si>
+  <si>
+    <t>theoreticalInsight_Final</t>
+  </si>
+  <si>
+    <t>externalEvent_Final</t>
+  </si>
+  <si>
+    <t>ForecastisUpdated</t>
+  </si>
+  <si>
+    <t>Percentage of team members who indicated their gender was either Female or Other, divided by team size</t>
+  </si>
+  <si>
+    <t>Percentage of team members who indicated their level of education was not PhD, divided by team size</t>
+  </si>
+  <si>
+    <t>Average age of team members who reported their age.</t>
+  </si>
+  <si>
+    <t>Percentage of team members who indicated their country of residence was not the United States, divided by team size</t>
+  </si>
+  <si>
+    <t>Number of distinct counterfactuals mentioned in submission</t>
+  </si>
+  <si>
+    <t>Indicates the indidividual number of entities that the submission placed holds responsible for the counterfactual.</t>
+  </si>
+  <si>
+    <t>0 = no mention, 1 = mentions updated data</t>
+  </si>
+  <si>
+    <t>0 = no mention, 1 = mentions theoretical insights</t>
+  </si>
+  <si>
+    <t>0 = no mention, 1 = mentions external event</t>
+  </si>
+  <si>
+    <t>Indicates whether the team mentioned the updated data as the reason/basis for their updated prediction</t>
+  </si>
+  <si>
+    <t>Indicates whether the team mentioned a theoretical insight as the reason/basis for their updated prediction</t>
+  </si>
+  <si>
+    <t>Indicates whether the team mentioned one or more external events as the reason/basis for their updated prediction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -900,6 +963,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1247,10 +1316,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEA65C1-8882-443D-817E-6C0B47AAF061}">
-  <dimension ref="A1:E200"/>
+  <dimension ref="A1:E196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J115" sqref="J115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,41 +1771,41 @@
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>240</v>
+      </c>
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B27" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B29" t="s">
         <v>73</v>
@@ -1745,15 +1814,15 @@
         <v>73</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B30" t="s">
         <v>73</v>
@@ -1762,15 +1831,15 @@
         <v>73</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B31" t="s">
         <v>73</v>
@@ -1779,10 +1848,10 @@
         <v>73</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1796,7 +1865,7 @@
         <v>73</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>129</v>
@@ -2144,7 +2213,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B59" t="s">
         <v>74</v>
@@ -2153,15 +2222,15 @@
         <v>73</v>
       </c>
       <c r="D59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B60" t="s">
         <v>74</v>
@@ -2170,15 +2239,15 @@
         <v>73</v>
       </c>
       <c r="D60" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B61" t="s">
         <v>74</v>
@@ -2187,7 +2256,7 @@
         <v>73</v>
       </c>
       <c r="D61" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E61" t="s">
         <v>142</v>
@@ -2195,7 +2264,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B62" t="s">
         <v>74</v>
@@ -2204,10 +2273,10 @@
         <v>73</v>
       </c>
       <c r="D62" t="s">
+        <v>260</v>
+      </c>
+      <c r="E62" t="s">
         <v>261</v>
-      </c>
-      <c r="E62" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2227,43 +2296,40 @@
         <v>226</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>147</v>
+        <v>102</v>
       </c>
       <c r="E64" t="s">
-        <v>148</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C65" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E65" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B66" t="s">
         <v>75</v>
@@ -2271,13 +2337,16 @@
       <c r="C66" t="s">
         <v>102</v>
       </c>
+      <c r="D66" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="E66" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B67" t="s">
         <v>75</v>
@@ -2286,15 +2355,15 @@
         <v>102</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E67" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B68" t="s">
         <v>75</v>
@@ -2302,16 +2371,16 @@
       <c r="C68" t="s">
         <v>102</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E68" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>157</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B69" t="s">
         <v>75</v>
@@ -2320,15 +2389,15 @@
         <v>102</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>156</v>
+        <v>77</v>
+      </c>
+      <c r="E69" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B70" t="s">
         <v>75</v>
@@ -2336,16 +2405,16 @@
       <c r="C70" t="s">
         <v>102</v>
       </c>
-      <c r="D70" t="s">
-        <v>157</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D70" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E70" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B71" t="s">
         <v>75</v>
@@ -2354,15 +2423,15 @@
         <v>102</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>77</v>
+        <v>162</v>
       </c>
       <c r="E71" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B72" t="s">
         <v>75</v>
@@ -2370,16 +2439,13 @@
       <c r="C72" t="s">
         <v>102</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="E72" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B73" t="s">
         <v>75</v>
@@ -2388,15 +2454,15 @@
         <v>102</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E73" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B74" t="s">
         <v>75</v>
@@ -2404,13 +2470,16 @@
       <c r="C74" t="s">
         <v>102</v>
       </c>
+      <c r="D74" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="E74" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>64</v>
+        <v>237</v>
       </c>
       <c r="B75" t="s">
         <v>75</v>
@@ -2419,98 +2488,92 @@
         <v>102</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>165</v>
+        <v>238</v>
       </c>
       <c r="E75" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B76" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E76" t="s">
-        <v>167</v>
+        <v>143</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>238</v>
+        <v>53</v>
       </c>
       <c r="B77" t="s">
+        <v>73</v>
+      </c>
+      <c r="C77" t="s">
+        <v>73</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E77" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>235</v>
+      </c>
+      <c r="B78" t="s">
         <v>75</v>
       </c>
-      <c r="C77" t="s">
-        <v>102</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E77" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>52</v>
-      </c>
-      <c r="B78" t="s">
-        <v>73</v>
-      </c>
       <c r="C78" t="s">
-        <v>73</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>144</v>
+        <v>102</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="B79" t="s">
         <v>73</v>
       </c>
       <c r="C79" t="s">
-        <v>73</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="E79" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>236</v>
+        <v>170</v>
       </c>
       <c r="B80" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C80" t="s">
         <v>102</v>
       </c>
-      <c r="D80" s="1"/>
       <c r="E80" t="s">
-        <v>237</v>
+        <v>171</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B81" t="s">
         <v>73</v>
@@ -2519,12 +2582,12 @@
         <v>102</v>
       </c>
       <c r="E81" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B82" t="s">
         <v>73</v>
@@ -2533,12 +2596,12 @@
         <v>102</v>
       </c>
       <c r="E82" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B83" t="s">
         <v>73</v>
@@ -2547,12 +2610,12 @@
         <v>102</v>
       </c>
       <c r="E83" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B84" t="s">
         <v>73</v>
@@ -2561,12 +2624,12 @@
         <v>102</v>
       </c>
       <c r="E84" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>176</v>
+        <v>68</v>
       </c>
       <c r="B85" t="s">
         <v>73</v>
@@ -2574,13 +2637,16 @@
       <c r="C85" t="s">
         <v>102</v>
       </c>
+      <c r="D85" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="E85" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>177</v>
+        <v>69</v>
       </c>
       <c r="B86" t="s">
         <v>73</v>
@@ -2588,13 +2654,16 @@
       <c r="C86" t="s">
         <v>102</v>
       </c>
+      <c r="D86" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="E86" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B87" t="s">
         <v>73</v>
@@ -2602,16 +2671,16 @@
       <c r="C87" t="s">
         <v>102</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>179</v>
+      <c r="D87" t="s">
+        <v>182</v>
       </c>
       <c r="E87" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B88" t="s">
         <v>73</v>
@@ -2619,16 +2688,16 @@
       <c r="C88" t="s">
         <v>102</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>179</v>
+      <c r="D88" t="s">
+        <v>184</v>
       </c>
       <c r="E88" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>70</v>
+        <v>186</v>
       </c>
       <c r="B89" t="s">
         <v>73</v>
@@ -2636,16 +2705,13 @@
       <c r="C89" t="s">
         <v>102</v>
       </c>
-      <c r="D89" t="s">
-        <v>182</v>
-      </c>
       <c r="E89" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>71</v>
+        <v>188</v>
       </c>
       <c r="B90" t="s">
         <v>73</v>
@@ -2653,16 +2719,13 @@
       <c r="C90" t="s">
         <v>102</v>
       </c>
-      <c r="D90" t="s">
-        <v>184</v>
-      </c>
       <c r="E90" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B91" t="s">
         <v>73</v>
@@ -2671,12 +2734,12 @@
         <v>102</v>
       </c>
       <c r="E91" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B92" t="s">
         <v>73</v>
@@ -2685,12 +2748,12 @@
         <v>102</v>
       </c>
       <c r="E92" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B93" t="s">
         <v>73</v>
@@ -2699,12 +2762,12 @@
         <v>102</v>
       </c>
       <c r="E93" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>192</v>
+        <v>91</v>
       </c>
       <c r="B94" t="s">
         <v>73</v>
@@ -2713,12 +2776,12 @@
         <v>102</v>
       </c>
       <c r="E94" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B95" t="s">
         <v>73</v>
@@ -2727,12 +2790,12 @@
         <v>102</v>
       </c>
       <c r="E95" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>91</v>
+        <v>198</v>
       </c>
       <c r="B96" t="s">
         <v>73</v>
@@ -2741,12 +2804,12 @@
         <v>102</v>
       </c>
       <c r="E96" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B97" t="s">
         <v>73</v>
@@ -2755,12 +2818,12 @@
         <v>102</v>
       </c>
       <c r="E97" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B98" t="s">
         <v>73</v>
@@ -2769,12 +2832,12 @@
         <v>102</v>
       </c>
       <c r="E98" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B99" t="s">
         <v>73</v>
@@ -2783,12 +2846,12 @@
         <v>102</v>
       </c>
       <c r="E99" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B100" t="s">
         <v>73</v>
@@ -2797,40 +2860,40 @@
         <v>102</v>
       </c>
       <c r="E100" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B101" t="s">
         <v>73</v>
       </c>
       <c r="C101" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E101" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B102" t="s">
         <v>73</v>
       </c>
       <c r="C102" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E102" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B103" t="s">
         <v>73</v>
@@ -2839,12 +2902,12 @@
         <v>116</v>
       </c>
       <c r="E103" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B104" t="s">
         <v>73</v>
@@ -2853,12 +2916,12 @@
         <v>116</v>
       </c>
       <c r="E104" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B105" t="s">
         <v>73</v>
@@ -2866,13 +2929,14 @@
       <c r="C105" t="s">
         <v>116</v>
       </c>
+      <c r="D105" s="1"/>
       <c r="E105" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B106" t="s">
         <v>73</v>
@@ -2880,13 +2944,14 @@
       <c r="C106" t="s">
         <v>116</v>
       </c>
+      <c r="D106" s="1"/>
       <c r="E106" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B107" t="s">
         <v>73</v>
@@ -2894,14 +2959,16 @@
       <c r="C107" t="s">
         <v>116</v>
       </c>
-      <c r="D107" s="1"/>
+      <c r="D107" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="E107" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B108" t="s">
         <v>73</v>
@@ -2909,14 +2976,16 @@
       <c r="C108" t="s">
         <v>116</v>
       </c>
-      <c r="D108" s="1"/>
+      <c r="D108" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="E108" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B109" t="s">
         <v>73</v>
@@ -2924,16 +2993,16 @@
       <c r="C109" t="s">
         <v>116</v>
       </c>
-      <c r="D109" s="1" t="s">
-        <v>179</v>
+      <c r="D109" t="s">
+        <v>182</v>
       </c>
       <c r="E109" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B110" t="s">
         <v>73</v>
@@ -2941,81 +3010,220 @@
       <c r="C110" t="s">
         <v>116</v>
       </c>
-      <c r="D110" s="1" t="s">
-        <v>179</v>
+      <c r="D110" t="s">
+        <v>184</v>
       </c>
       <c r="E110" t="s">
-        <v>181</v>
+        <v>223</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="B111" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C111" t="s">
-        <v>116</v>
-      </c>
-      <c r="D111" t="s">
-        <v>182</v>
+        <v>73</v>
       </c>
       <c r="E111" t="s">
-        <v>221</v>
+        <v>272</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>222</v>
+        <v>263</v>
       </c>
       <c r="B112" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C112" t="s">
-        <v>116</v>
-      </c>
-      <c r="D112" t="s">
-        <v>184</v>
+        <v>73</v>
       </c>
       <c r="E112" t="s">
-        <v>223</v>
+        <v>273</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>229</v>
+        <v>264</v>
       </c>
       <c r="B113" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C113" t="s">
         <v>73</v>
       </c>
-      <c r="D113" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="E113" t="s">
-        <v>231</v>
+        <v>274</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>232</v>
+        <v>265</v>
       </c>
       <c r="B114" t="s">
         <v>74</v>
       </c>
       <c r="C114" t="s">
+        <v>73</v>
+      </c>
+      <c r="E114" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>94</v>
+      </c>
+      <c r="B115" t="s">
+        <v>74</v>
+      </c>
+      <c r="C115" t="s">
+        <v>73</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E115" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>54</v>
+      </c>
+      <c r="B116" t="s">
+        <v>74</v>
+      </c>
+      <c r="C116" t="s">
+        <v>73</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E116" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>266</v>
+      </c>
+      <c r="B117" t="s">
+        <v>74</v>
+      </c>
+      <c r="C117" t="s">
+        <v>73</v>
+      </c>
+      <c r="E117" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>267</v>
+      </c>
+      <c r="B118" t="s">
+        <v>74</v>
+      </c>
+      <c r="C118" t="s">
+        <v>73</v>
+      </c>
+      <c r="E118" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>268</v>
+      </c>
+      <c r="B119" t="s">
+        <v>74</v>
+      </c>
+      <c r="C119" t="s">
+        <v>116</v>
+      </c>
+      <c r="D119" t="s">
+        <v>278</v>
+      </c>
+      <c r="E119" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>269</v>
+      </c>
+      <c r="B120" t="s">
+        <v>74</v>
+      </c>
+      <c r="C120" t="s">
+        <v>116</v>
+      </c>
+      <c r="D120" t="s">
+        <v>279</v>
+      </c>
+      <c r="E120" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>270</v>
+      </c>
+      <c r="B121" t="s">
+        <v>74</v>
+      </c>
+      <c r="C121" t="s">
+        <v>116</v>
+      </c>
+      <c r="D121" t="s">
+        <v>280</v>
+      </c>
+      <c r="E121" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>229</v>
+      </c>
+      <c r="B122" t="s">
+        <v>73</v>
+      </c>
+      <c r="C122" t="s">
+        <v>73</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E122" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>271</v>
+      </c>
+      <c r="B123" t="s">
+        <v>74</v>
+      </c>
+      <c r="C123" t="s">
+        <v>232</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="E123" t="s">
         <v>234</v>
       </c>
-      <c r="E114" t="s">
-        <v>235</v>
-      </c>
-    </row>
+    </row>
+    <row r="151" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="155" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="156" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="157" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3058,14 +3266,11 @@
     <row r="194" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="195" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="196" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D200">
-    <sortCondition ref="A8:A200"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D196">
+    <sortCondition ref="A8:A196"/>
   </sortState>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
number of parameters - academic
Add coded number of parameters for academic sample.
</commit_message>
<xml_diff>
--- a/Columns reference.xlsx
+++ b/Columns reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/ottwardu_uwaterloo_ca/Documents/Documents/GitHub/Forecasting-Tournament/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="13_ncr:1_{9F9CA9E6-EFA6-4D9B-8143-CA724CACC61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28BC619A-DF51-4206-A653-64BA1F905946}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="13_ncr:1_{9F9CA9E6-EFA6-4D9B-8143-CA724CACC61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8260C25B-9604-4126-B13D-E2D72EADC966}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BFB2704-2340-4873-B614-2DBCF2A7F097}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="287">
   <si>
     <t>Description</t>
   </si>
@@ -936,6 +936,15 @@
   </si>
   <si>
     <t>Indicates whether the team mentioned one or more external events as the reason/basis for their updated prediction</t>
+  </si>
+  <si>
+    <t># of parameters (coded)</t>
+  </si>
+  <si>
+    <t>parameters_coded</t>
+  </si>
+  <si>
+    <t>Coded number of parameters participant mentioned in the parameters and covidcondyn/covidmeas columns</t>
   </si>
 </sst>
 </file>
@@ -1318,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEA65C1-8882-443D-817E-6C0B47AAF061}">
   <dimension ref="A1:E196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J115" sqref="J115"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3218,6 +3227,23 @@
       </c>
       <c r="E123" t="s">
         <v>234</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>285</v>
+      </c>
+      <c r="B124" t="s">
+        <v>74</v>
+      </c>
+      <c r="C124" t="s">
+        <v>73</v>
+      </c>
+      <c r="D124" t="s">
+        <v>284</v>
+      </c>
+      <c r="E124" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="151" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added missing lay people codes for number of parameters
</commit_message>
<xml_diff>
--- a/Columns reference.xlsx
+++ b/Columns reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/ottwardu_uwaterloo_ca/Documents/Documents/GitHub/Forecasting-Tournament/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="13_ncr:1_{9F9CA9E6-EFA6-4D9B-8143-CA724CACC61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8260C25B-9604-4126-B13D-E2D72EADC966}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{9F9CA9E6-EFA6-4D9B-8143-CA724CACC61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CC00B15-B94F-4A14-8BEB-8BBC43C3DA15}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BFB2704-2340-4873-B614-2DBCF2A7F097}"/>
   </bookViews>
@@ -902,18 +902,9 @@
     <t>ForecastisUpdated</t>
   </si>
   <si>
-    <t>Percentage of team members who indicated their gender was either Female or Other, divided by team size</t>
-  </si>
-  <si>
-    <t>Percentage of team members who indicated their level of education was not PhD, divided by team size</t>
-  </si>
-  <si>
     <t>Average age of team members who reported their age.</t>
   </si>
   <si>
-    <t>Percentage of team members who indicated their country of residence was not the United States, divided by team size</t>
-  </si>
-  <si>
     <t>Number of distinct counterfactuals mentioned in submission</t>
   </si>
   <si>
@@ -945,6 +936,15 @@
   </si>
   <si>
     <t>Coded number of parameters participant mentioned in the parameters and covidcondyn/covidmeas columns</t>
+  </si>
+  <si>
+    <t>Percentage of team members who indicated their gender was either Female or Other</t>
+  </si>
+  <si>
+    <t>Percentage of team members who indicated their level of education was not PhD</t>
+  </si>
+  <si>
+    <t>Percentage of team members who indicated their country of residence was not the United States</t>
   </si>
 </sst>
 </file>
@@ -1327,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEA65C1-8882-443D-817E-6C0B47AAF061}">
   <dimension ref="A1:E196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="E126" sqref="E126"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E114" sqref="E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3037,7 +3037,7 @@
         <v>73</v>
       </c>
       <c r="E111" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3051,7 +3051,7 @@
         <v>73</v>
       </c>
       <c r="E112" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3065,7 +3065,7 @@
         <v>73</v>
       </c>
       <c r="E113" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3079,7 +3079,7 @@
         <v>73</v>
       </c>
       <c r="E114" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3127,7 +3127,7 @@
         <v>73</v>
       </c>
       <c r="E117" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3141,7 +3141,7 @@
         <v>73</v>
       </c>
       <c r="E118" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3155,10 +3155,10 @@
         <v>116</v>
       </c>
       <c r="D119" t="s">
+        <v>275</v>
+      </c>
+      <c r="E119" t="s">
         <v>278</v>
-      </c>
-      <c r="E119" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3172,10 +3172,10 @@
         <v>116</v>
       </c>
       <c r="D120" t="s">
+        <v>276</v>
+      </c>
+      <c r="E120" t="s">
         <v>279</v>
-      </c>
-      <c r="E120" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3189,10 +3189,10 @@
         <v>116</v>
       </c>
       <c r="D121" t="s">
+        <v>277</v>
+      </c>
+      <c r="E121" t="s">
         <v>280</v>
-      </c>
-      <c r="E121" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3231,7 +3231,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B124" t="s">
         <v>74</v>
@@ -3240,10 +3240,10 @@
         <v>73</v>
       </c>
       <c r="D124" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E124" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="151" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added corrected review justification + re-added gender identity column for prolific sample
</commit_message>
<xml_diff>
--- a/Columns reference.xlsx
+++ b/Columns reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/ottwardu_uwaterloo_ca/Documents/Documents/GitHub/Forecasting-Tournament/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{9F9CA9E6-EFA6-4D9B-8143-CA724CACC61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CC00B15-B94F-4A14-8BEB-8BBC43C3DA15}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="13_ncr:1_{9F9CA9E6-EFA6-4D9B-8143-CA724CACC61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9010171F-D254-43E4-8CCF-5D51B04DF033}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BFB2704-2340-4873-B614-2DBCF2A7F097}"/>
   </bookViews>
@@ -890,15 +890,6 @@
     <t>counterNum</t>
   </si>
   <si>
-    <t>dataReceived_Final</t>
-  </si>
-  <si>
-    <t>theoreticalInsight_Final</t>
-  </si>
-  <si>
-    <t>externalEvent_Final</t>
-  </si>
-  <si>
     <t>ForecastisUpdated</t>
   </si>
   <si>
@@ -945,6 +936,15 @@
   </si>
   <si>
     <t>Percentage of team members who indicated their country of residence was not the United States</t>
+  </si>
+  <si>
+    <t>justification_dataReceived</t>
+  </si>
+  <si>
+    <t>justification_theoreticalInsight</t>
+  </si>
+  <si>
+    <t>justification_externalEvent</t>
   </si>
 </sst>
 </file>
@@ -1327,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEA65C1-8882-443D-817E-6C0B47AAF061}">
   <dimension ref="A1:E196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="E114" sqref="E114"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3037,7 +3037,7 @@
         <v>73</v>
       </c>
       <c r="E111" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3051,7 +3051,7 @@
         <v>73</v>
       </c>
       <c r="E112" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3065,7 +3065,7 @@
         <v>73</v>
       </c>
       <c r="E113" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3079,7 +3079,7 @@
         <v>73</v>
       </c>
       <c r="E114" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3127,7 +3127,7 @@
         <v>73</v>
       </c>
       <c r="E117" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3141,12 +3141,12 @@
         <v>73</v>
       </c>
       <c r="E118" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="B119" t="s">
         <v>74</v>
@@ -3155,15 +3155,15 @@
         <v>116</v>
       </c>
       <c r="D119" t="s">
+        <v>272</v>
+      </c>
+      <c r="E119" t="s">
         <v>275</v>
-      </c>
-      <c r="E119" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="B120" t="s">
         <v>74</v>
@@ -3172,15 +3172,15 @@
         <v>116</v>
       </c>
       <c r="D120" t="s">
+        <v>273</v>
+      </c>
+      <c r="E120" t="s">
         <v>276</v>
-      </c>
-      <c r="E120" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="B121" t="s">
         <v>74</v>
@@ -3189,10 +3189,10 @@
         <v>116</v>
       </c>
       <c r="D121" t="s">
+        <v>274</v>
+      </c>
+      <c r="E121" t="s">
         <v>277</v>
-      </c>
-      <c r="E121" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3214,7 +3214,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B123" t="s">
         <v>74</v>
@@ -3231,7 +3231,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B124" t="s">
         <v>74</v>
@@ -3240,10 +3240,10 @@
         <v>73</v>
       </c>
       <c r="D124" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E124" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="151" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed definitions in legend file for mean absolute percentage error columns
</commit_message>
<xml_diff>
--- a/Columns reference.xlsx
+++ b/Columns reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/ottwardu_uwaterloo_ca/Documents/Documents/GitHub/Forecasting-Tournament/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="13_ncr:1_{9F9CA9E6-EFA6-4D9B-8143-CA724CACC61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9010171F-D254-43E4-8CCF-5D51B04DF033}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="13_ncr:1_{9F9CA9E6-EFA6-4D9B-8143-CA724CACC61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A11A8A20-C8B9-41F3-94B8-33A49ECDB045}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BFB2704-2340-4873-B614-2DBCF2A7F097}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="287">
   <si>
     <t>Description</t>
   </si>
@@ -797,15 +797,6 @@
     <t>difference between the last click - first click participants made when on the submission page for each domain, indicating how long they spent on each submission.</t>
   </si>
   <si>
-    <t>flag_lay_responses</t>
-  </si>
-  <si>
-    <t>1 = flagged, 0/NA = no issue</t>
-  </si>
-  <si>
-    <t>coding variable that indicated Prolific responses that were flagged by coders. Those flagged as 1s have been removed</t>
-  </si>
-  <si>
     <t>basis</t>
   </si>
   <si>
@@ -945,6 +936,15 @@
   </si>
   <si>
     <t>justification_externalEvent</t>
+  </si>
+  <si>
+    <t>Mean Absolute Percentage Error for phase 1 COVID predictions (Months 1-12)</t>
+  </si>
+  <si>
+    <t>Mean Absolute Percentage Error  for phase 1 predictions (Months 7-12)</t>
+  </si>
+  <si>
+    <t>Mean Absolute Percentage Error for phase 2 predictions (Months 7-12)</t>
   </si>
 </sst>
 </file>
@@ -1325,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEA65C1-8882-443D-817E-6C0B47AAF061}">
-  <dimension ref="A1:E196"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B27" t="s">
         <v>73</v>
@@ -1789,15 +1789,15 @@
         <v>73</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B28" t="s">
         <v>73</v>
@@ -1806,61 +1806,61 @@
         <v>73</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>243</v>
+      </c>
+      <c r="B29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="B29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>244</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="B30" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>245</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="B31" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1874,7 +1874,7 @@
         <v>73</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>129</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B59" t="s">
         <v>74</v>
@@ -2231,15 +2231,15 @@
         <v>73</v>
       </c>
       <c r="D59" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E59" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B60" t="s">
         <v>74</v>
@@ -2248,15 +2248,15 @@
         <v>73</v>
       </c>
       <c r="D60" t="s">
+        <v>251</v>
+      </c>
+      <c r="E60" t="s">
         <v>254</v>
-      </c>
-      <c r="E60" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B61" t="s">
         <v>74</v>
@@ -2265,7 +2265,7 @@
         <v>73</v>
       </c>
       <c r="D61" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E61" t="s">
         <v>142</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B62" t="s">
         <v>74</v>
@@ -2282,10 +2282,10 @@
         <v>73</v>
       </c>
       <c r="D62" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E62" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2486,26 +2486,26 @@
         <v>167</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>237</v>
+        <v>52</v>
       </c>
       <c r="B75" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E75" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B76" t="s">
         <v>73</v>
@@ -2514,47 +2514,44 @@
         <v>73</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
+      </c>
+      <c r="E76" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>53</v>
+        <v>235</v>
       </c>
       <c r="B77" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>73</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>145</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="D77" s="1"/>
       <c r="E77" t="s">
-        <v>146</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>235</v>
+        <v>168</v>
       </c>
       <c r="B78" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C78" t="s">
         <v>102</v>
       </c>
-      <c r="D78" s="1"/>
       <c r="E78" t="s">
-        <v>236</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B79" t="s">
         <v>73</v>
@@ -2563,12 +2560,12 @@
         <v>102</v>
       </c>
       <c r="E79" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B80" t="s">
         <v>73</v>
@@ -2577,12 +2574,12 @@
         <v>102</v>
       </c>
       <c r="E80" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B81" t="s">
         <v>73</v>
@@ -2591,12 +2588,12 @@
         <v>102</v>
       </c>
       <c r="E81" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B82" t="s">
         <v>73</v>
@@ -2605,12 +2602,12 @@
         <v>102</v>
       </c>
       <c r="E82" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B83" t="s">
         <v>73</v>
@@ -2619,12 +2616,12 @@
         <v>102</v>
       </c>
       <c r="E83" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>177</v>
+        <v>68</v>
       </c>
       <c r="B84" t="s">
         <v>73</v>
@@ -2632,13 +2629,16 @@
       <c r="C84" t="s">
         <v>102</v>
       </c>
+      <c r="D84" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="E84" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B85" t="s">
         <v>73</v>
@@ -2650,12 +2650,12 @@
         <v>179</v>
       </c>
       <c r="E85" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B86" t="s">
         <v>73</v>
@@ -2663,16 +2663,16 @@
       <c r="C86" t="s">
         <v>102</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>179</v>
+      <c r="D86" t="s">
+        <v>182</v>
       </c>
       <c r="E86" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B87" t="s">
         <v>73</v>
@@ -2681,15 +2681,15 @@
         <v>102</v>
       </c>
       <c r="D87" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E87" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>71</v>
+        <v>186</v>
       </c>
       <c r="B88" t="s">
         <v>73</v>
@@ -2697,16 +2697,13 @@
       <c r="C88" t="s">
         <v>102</v>
       </c>
-      <c r="D88" t="s">
-        <v>184</v>
-      </c>
       <c r="E88" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B89" t="s">
         <v>73</v>
@@ -2715,12 +2712,12 @@
         <v>102</v>
       </c>
       <c r="E89" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B90" t="s">
         <v>73</v>
@@ -2729,12 +2726,12 @@
         <v>102</v>
       </c>
       <c r="E90" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B91" t="s">
         <v>73</v>
@@ -2743,12 +2740,12 @@
         <v>102</v>
       </c>
       <c r="E91" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B92" t="s">
         <v>73</v>
@@ -2757,12 +2754,12 @@
         <v>102</v>
       </c>
       <c r="E92" t="s">
-        <v>193</v>
+        <v>284</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>194</v>
+        <v>91</v>
       </c>
       <c r="B93" t="s">
         <v>73</v>
@@ -2771,12 +2768,12 @@
         <v>102</v>
       </c>
       <c r="E93" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>91</v>
+        <v>196</v>
       </c>
       <c r="B94" t="s">
         <v>73</v>
@@ -2785,12 +2782,12 @@
         <v>102</v>
       </c>
       <c r="E94" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B95" t="s">
         <v>73</v>
@@ -2799,12 +2796,12 @@
         <v>102</v>
       </c>
       <c r="E95" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B96" t="s">
         <v>73</v>
@@ -2813,12 +2810,12 @@
         <v>102</v>
       </c>
       <c r="E96" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B97" t="s">
         <v>73</v>
@@ -2827,12 +2824,12 @@
         <v>102</v>
       </c>
       <c r="E97" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B98" t="s">
         <v>73</v>
@@ -2841,12 +2838,12 @@
         <v>102</v>
       </c>
       <c r="E98" t="s">
-        <v>203</v>
+        <v>285</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B99" t="s">
         <v>73</v>
@@ -2855,26 +2852,26 @@
         <v>102</v>
       </c>
       <c r="E99" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B100" t="s">
         <v>73</v>
       </c>
       <c r="C100" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E100" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B101" t="s">
         <v>73</v>
@@ -2883,12 +2880,12 @@
         <v>116</v>
       </c>
       <c r="E101" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B102" t="s">
         <v>73</v>
@@ -2897,12 +2894,12 @@
         <v>116</v>
       </c>
       <c r="E102" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B103" t="s">
         <v>73</v>
@@ -2911,12 +2908,12 @@
         <v>116</v>
       </c>
       <c r="E103" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B104" t="s">
         <v>73</v>
@@ -2924,13 +2921,14 @@
       <c r="C104" t="s">
         <v>116</v>
       </c>
+      <c r="D104" s="1"/>
       <c r="E104" t="s">
-        <v>214</v>
+        <v>286</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B105" t="s">
         <v>73</v>
@@ -2940,12 +2938,12 @@
       </c>
       <c r="D105" s="1"/>
       <c r="E105" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B106" t="s">
         <v>73</v>
@@ -2953,14 +2951,16 @@
       <c r="C106" t="s">
         <v>116</v>
       </c>
-      <c r="D106" s="1"/>
+      <c r="D106" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="E106" t="s">
-        <v>217</v>
+        <v>180</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B107" t="s">
         <v>73</v>
@@ -2972,12 +2972,12 @@
         <v>179</v>
       </c>
       <c r="E107" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B108" t="s">
         <v>73</v>
@@ -2985,16 +2985,16 @@
       <c r="C108" t="s">
         <v>116</v>
       </c>
-      <c r="D108" s="1" t="s">
-        <v>179</v>
+      <c r="D108" t="s">
+        <v>182</v>
       </c>
       <c r="E108" t="s">
-        <v>181</v>
+        <v>221</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B109" t="s">
         <v>73</v>
@@ -3003,32 +3003,29 @@
         <v>116</v>
       </c>
       <c r="D109" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E109" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>222</v>
+        <v>259</v>
       </c>
       <c r="B110" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C110" t="s">
-        <v>116</v>
-      </c>
-      <c r="D110" t="s">
-        <v>184</v>
+        <v>73</v>
       </c>
       <c r="E110" t="s">
-        <v>223</v>
+        <v>278</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B111" t="s">
         <v>74</v>
@@ -3037,12 +3034,12 @@
         <v>73</v>
       </c>
       <c r="E111" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B112" t="s">
         <v>74</v>
@@ -3051,12 +3048,12 @@
         <v>73</v>
       </c>
       <c r="E112" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B113" t="s">
         <v>74</v>
@@ -3065,12 +3062,12 @@
         <v>73</v>
       </c>
       <c r="E113" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>265</v>
+        <v>94</v>
       </c>
       <c r="B114" t="s">
         <v>74</v>
@@ -3078,13 +3075,16 @@
       <c r="C114" t="s">
         <v>73</v>
       </c>
+      <c r="D114" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="E114" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="B115" t="s">
         <v>74</v>
@@ -3093,15 +3093,15 @@
         <v>73</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E115" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>54</v>
+        <v>263</v>
       </c>
       <c r="B116" t="s">
         <v>74</v>
@@ -3109,16 +3109,13 @@
       <c r="C116" t="s">
         <v>73</v>
       </c>
-      <c r="D116" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="E116" t="s">
-        <v>150</v>
+        <v>268</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B117" t="s">
         <v>74</v>
@@ -3127,26 +3124,29 @@
         <v>73</v>
       </c>
       <c r="E117" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
       <c r="B118" t="s">
         <v>74</v>
       </c>
       <c r="C118" t="s">
-        <v>73</v>
+        <v>116</v>
+      </c>
+      <c r="D118" t="s">
+        <v>269</v>
       </c>
       <c r="E118" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B119" t="s">
         <v>74</v>
@@ -3155,15 +3155,15 @@
         <v>116</v>
       </c>
       <c r="D119" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E119" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B120" t="s">
         <v>74</v>
@@ -3172,80 +3172,64 @@
         <v>116</v>
       </c>
       <c r="D120" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E120" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>286</v>
+        <v>229</v>
       </c>
       <c r="B121" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C121" t="s">
-        <v>116</v>
-      </c>
-      <c r="D121" t="s">
-        <v>274</v>
+        <v>73</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="E121" t="s">
-        <v>277</v>
+        <v>231</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>229</v>
+        <v>265</v>
       </c>
       <c r="B122" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C122" t="s">
-        <v>73</v>
+        <v>232</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E122" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="B123" t="s">
         <v>74</v>
       </c>
       <c r="C123" t="s">
-        <v>232</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>233</v>
+        <v>73</v>
+      </c>
+      <c r="D123" t="s">
+        <v>275</v>
       </c>
       <c r="E123" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>279</v>
-      </c>
-      <c r="B124" t="s">
-        <v>74</v>
-      </c>
-      <c r="C124" t="s">
-        <v>73</v>
-      </c>
-      <c r="D124" t="s">
-        <v>278</v>
-      </c>
-      <c r="E124" t="s">
-        <v>280</v>
-      </c>
-    </row>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="150" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="151" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="152" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="153" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3291,10 +3275,9 @@
     <row r="193" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="194" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="195" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D196">
-    <sortCondition ref="A8:A196"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D195">
+    <sortCondition ref="A8:A195"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
umain overhaul of analyses and additional stats
added data files from the other branch (because merging does not work), added back snipped for creating mase for the first 6 month of t1, added column ref from the other branch, and made progress on marking and commenting the main analyses (still work in progress but almost there)
</commit_message>
<xml_diff>
--- a/Columns reference.xlsx
+++ b/Columns reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/ottwardu_uwaterloo_ca/Documents/Documents/GitHub/Forecasting-Tournament/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igrossma\Documents\GitHub\Forecasting-Tournament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="13_ncr:1_{9F9CA9E6-EFA6-4D9B-8143-CA724CACC61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A11A8A20-C8B9-41F3-94B8-33A49ECDB045}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE98E6A4-37C2-4797-8DFC-419010B0DB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BFB2704-2340-4873-B614-2DBCF2A7F097}"/>
+    <workbookView xWindow="880" yWindow="690" windowWidth="14400" windowHeight="7360" xr2:uid="{3BFB2704-2340-4873-B614-2DBCF2A7F097}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -318,9 +318,6 @@
     <t>1 = phase 1, 2 = phase 2</t>
   </si>
   <si>
-    <t>CounterFactual_Presence.Final</t>
-  </si>
-  <si>
     <t>Column Name</t>
   </si>
   <si>
@@ -945,6 +942,9 @@
   </si>
   <si>
     <t>Mean Absolute Percentage Error for phase 2 predictions (Months 7-12)</t>
+  </si>
+  <si>
+    <t>CounterFactual_Presence_Final</t>
   </si>
 </sst>
 </file>
@@ -1327,21 +1327,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEA65C1-8882-443D-817E-6C0B47AAF061}">
   <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.26953125" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" customWidth="1"/>
+    <col min="4" max="4" width="45.81640625" customWidth="1"/>
+    <col min="5" max="5" width="56.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1356,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1367,13 +1367,13 @@
         <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1384,10 +1384,10 @@
         <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1398,13 +1398,13 @@
         <v>73</v>
       </c>
       <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
         <v>98</v>
       </c>
-      <c r="E4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" ht="192" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1415,13 +1415,13 @@
         <v>73</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1429,16 +1429,16 @@
         <v>73</v>
       </c>
       <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1446,16 +1446,16 @@
         <v>73</v>
       </c>
       <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1463,16 +1463,16 @@
         <v>73</v>
       </c>
       <c r="C8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1480,16 +1480,16 @@
         <v>73</v>
       </c>
       <c r="C9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1497,16 +1497,16 @@
         <v>73</v>
       </c>
       <c r="C10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1514,16 +1514,16 @@
         <v>73</v>
       </c>
       <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1534,13 +1534,13 @@
         <v>73</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1551,13 +1551,13 @@
         <v>73</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1568,13 +1568,13 @@
         <v>73</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1585,13 +1585,13 @@
         <v>73</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1602,13 +1602,13 @@
         <v>73</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1619,13 +1619,13 @@
         <v>73</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1633,16 +1633,16 @@
         <v>74</v>
       </c>
       <c r="C18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1650,16 +1650,16 @@
         <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1667,16 +1667,16 @@
         <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1684,16 +1684,16 @@
         <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1701,16 +1701,16 @@
         <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1718,16 +1718,16 @@
         <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -1738,13 +1738,13 @@
         <v>73</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1755,13 +1755,13 @@
         <v>73</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" t="s">
         <v>125</v>
       </c>
-      <c r="E25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1772,98 +1772,98 @@
         <v>73</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B27" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E27" s="1" t="s">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E28" s="1" t="s">
+    </row>
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>243</v>
       </c>
-      <c r="B29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>244</v>
       </c>
-      <c r="B30" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>245</v>
-      </c>
-      <c r="B31" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -1874,13 +1874,13 @@
         <v>73</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -1891,13 +1891,13 @@
         <v>73</v>
       </c>
       <c r="D33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1908,13 +1908,13 @@
         <v>73</v>
       </c>
       <c r="D34" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1922,13 +1922,13 @@
         <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1936,13 +1936,13 @@
         <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1950,13 +1950,13 @@
         <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1964,13 +1964,13 @@
         <v>73</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1978,13 +1978,13 @@
         <v>73</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1992,13 +1992,13 @@
         <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -2006,13 +2006,13 @@
         <v>73</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -2020,13 +2020,13 @@
         <v>73</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -2034,13 +2034,13 @@
         <v>73</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -2048,13 +2048,13 @@
         <v>73</v>
       </c>
       <c r="C44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -2062,13 +2062,13 @@
         <v>73</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -2076,13 +2076,13 @@
         <v>73</v>
       </c>
       <c r="C46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -2093,38 +2093,38 @@
         <v>73</v>
       </c>
       <c r="D47" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E47" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -2135,13 +2135,13 @@
         <v>73</v>
       </c>
       <c r="D53" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -2155,10 +2155,10 @@
         <v>93</v>
       </c>
       <c r="E54" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -2169,13 +2169,13 @@
         <v>73</v>
       </c>
       <c r="D55" t="s">
+        <v>136</v>
+      </c>
+      <c r="E55" t="s">
         <v>137</v>
       </c>
-      <c r="E55" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -2186,13 +2186,13 @@
         <v>73</v>
       </c>
       <c r="D56" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E56" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>50</v>
       </c>
@@ -2203,10 +2203,10 @@
         <v>73</v>
       </c>
       <c r="E57" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -2217,12 +2217,12 @@
         <v>73</v>
       </c>
       <c r="E58" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B59" t="s">
         <v>74</v>
@@ -2231,15 +2231,15 @@
         <v>73</v>
       </c>
       <c r="D59" t="s">
+        <v>250</v>
+      </c>
+      <c r="E59" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>251</v>
-      </c>
-      <c r="E59" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>252</v>
       </c>
       <c r="B60" t="s">
         <v>74</v>
@@ -2248,15 +2248,15 @@
         <v>73</v>
       </c>
       <c r="D60" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E60" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>255</v>
       </c>
       <c r="B61" t="s">
         <v>74</v>
@@ -2265,15 +2265,15 @@
         <v>73</v>
       </c>
       <c r="D61" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E61" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B62" t="s">
         <v>74</v>
@@ -2282,30 +2282,30 @@
         <v>73</v>
       </c>
       <c r="D62" t="s">
+        <v>256</v>
+      </c>
+      <c r="E62" t="s">
         <v>257</v>
       </c>
-      <c r="E62" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>223</v>
+      </c>
+      <c r="B63" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" t="s">
+        <v>73</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B63" t="s">
-        <v>73</v>
-      </c>
-      <c r="C63" t="s">
-        <v>73</v>
-      </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" t="s">
         <v>225</v>
       </c>
-      <c r="E63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -2313,13 +2313,13 @@
         <v>75</v>
       </c>
       <c r="C64" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E64" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>56</v>
       </c>
@@ -2327,16 +2327,16 @@
         <v>75</v>
       </c>
       <c r="C65" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D65" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E65" t="s">
         <v>151</v>
       </c>
-      <c r="E65" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>57</v>
       </c>
@@ -2344,16 +2344,16 @@
         <v>75</v>
       </c>
       <c r="C66" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D66" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E66" t="s">
         <v>153</v>
       </c>
-      <c r="E66" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>58</v>
       </c>
@@ -2361,16 +2361,16 @@
         <v>75</v>
       </c>
       <c r="C67" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D67" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>59</v>
       </c>
@@ -2378,16 +2378,16 @@
         <v>75</v>
       </c>
       <c r="C68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D68" t="s">
+        <v>156</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>60</v>
       </c>
@@ -2395,16 +2395,16 @@
         <v>75</v>
       </c>
       <c r="C69" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E69" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>61</v>
       </c>
@@ -2412,16 +2412,16 @@
         <v>75</v>
       </c>
       <c r="C70" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D70" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E70" t="s">
         <v>160</v>
       </c>
-      <c r="E70" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>62</v>
       </c>
@@ -2429,16 +2429,16 @@
         <v>75</v>
       </c>
       <c r="C71" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D71" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E71" t="s">
         <v>162</v>
       </c>
-      <c r="E71" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>63</v>
       </c>
@@ -2446,13 +2446,13 @@
         <v>75</v>
       </c>
       <c r="C72" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E72" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>64</v>
       </c>
@@ -2460,16 +2460,16 @@
         <v>75</v>
       </c>
       <c r="C73" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D73" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E73" t="s">
         <v>165</v>
       </c>
-      <c r="E73" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>65</v>
       </c>
@@ -2477,16 +2477,16 @@
         <v>75</v>
       </c>
       <c r="C74" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E74" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>52</v>
       </c>
@@ -2497,13 +2497,13 @@
         <v>73</v>
       </c>
       <c r="D75" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E75" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>53</v>
       </c>
@@ -2514,112 +2514,112 @@
         <v>73</v>
       </c>
       <c r="D76" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E76" t="s">
         <v>145</v>
       </c>
-      <c r="E76" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B77" t="s">
         <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
+        <v>167</v>
+      </c>
+      <c r="B78" t="s">
+        <v>73</v>
+      </c>
+      <c r="C78" t="s">
+        <v>101</v>
+      </c>
+      <c r="E78" t="s">
         <v>168</v>
       </c>
-      <c r="B78" t="s">
-        <v>73</v>
-      </c>
-      <c r="C78" t="s">
-        <v>102</v>
-      </c>
-      <c r="E78" t="s">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="B79" t="s">
+        <v>73</v>
+      </c>
+      <c r="C79" t="s">
+        <v>101</v>
+      </c>
+      <c r="E79" t="s">
         <v>170</v>
       </c>
-      <c r="B79" t="s">
-        <v>73</v>
-      </c>
-      <c r="C79" t="s">
-        <v>102</v>
-      </c>
-      <c r="E79" t="s">
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="B80" t="s">
+        <v>73</v>
+      </c>
+      <c r="C80" t="s">
+        <v>101</v>
+      </c>
+      <c r="E80" t="s">
         <v>172</v>
       </c>
-      <c r="B80" t="s">
-        <v>73</v>
-      </c>
-      <c r="C80" t="s">
-        <v>102</v>
-      </c>
-      <c r="E80" t="s">
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="B81" t="s">
+        <v>73</v>
+      </c>
+      <c r="C81" t="s">
+        <v>101</v>
+      </c>
+      <c r="E81" t="s">
         <v>174</v>
       </c>
-      <c r="B81" t="s">
-        <v>73</v>
-      </c>
-      <c r="C81" t="s">
-        <v>102</v>
-      </c>
-      <c r="E81" t="s">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="B82" t="s">
+        <v>73</v>
+      </c>
+      <c r="C82" t="s">
+        <v>101</v>
+      </c>
+      <c r="E82" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>176</v>
       </c>
-      <c r="B82" t="s">
-        <v>73</v>
-      </c>
-      <c r="C82" t="s">
-        <v>102</v>
-      </c>
-      <c r="E82" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="B83" t="s">
+        <v>73</v>
+      </c>
+      <c r="C83" t="s">
+        <v>101</v>
+      </c>
+      <c r="E83" t="s">
         <v>177</v>
       </c>
-      <c r="B83" t="s">
-        <v>73</v>
-      </c>
-      <c r="C83" t="s">
-        <v>102</v>
-      </c>
-      <c r="E83" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>68</v>
       </c>
@@ -2627,16 +2627,16 @@
         <v>73</v>
       </c>
       <c r="C84" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D84" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E84" t="s">
         <v>179</v>
       </c>
-      <c r="E84" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>69</v>
       </c>
@@ -2644,16 +2644,16 @@
         <v>73</v>
       </c>
       <c r="C85" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E85" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>70</v>
       </c>
@@ -2661,16 +2661,16 @@
         <v>73</v>
       </c>
       <c r="C86" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D86" t="s">
+        <v>181</v>
+      </c>
+      <c r="E86" t="s">
         <v>182</v>
       </c>
-      <c r="E86" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>71</v>
       </c>
@@ -2678,86 +2678,86 @@
         <v>73</v>
       </c>
       <c r="C87" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D87" t="s">
+        <v>183</v>
+      </c>
+      <c r="E87" t="s">
         <v>184</v>
       </c>
-      <c r="E87" t="s">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="B88" t="s">
+        <v>73</v>
+      </c>
+      <c r="C88" t="s">
+        <v>101</v>
+      </c>
+      <c r="E88" t="s">
         <v>186</v>
       </c>
-      <c r="B88" t="s">
-        <v>73</v>
-      </c>
-      <c r="C88" t="s">
-        <v>102</v>
-      </c>
-      <c r="E88" t="s">
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="B89" t="s">
+        <v>73</v>
+      </c>
+      <c r="C89" t="s">
+        <v>101</v>
+      </c>
+      <c r="E89" t="s">
         <v>188</v>
       </c>
-      <c r="B89" t="s">
-        <v>73</v>
-      </c>
-      <c r="C89" t="s">
-        <v>102</v>
-      </c>
-      <c r="E89" t="s">
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="B90" t="s">
+        <v>73</v>
+      </c>
+      <c r="C90" t="s">
+        <v>101</v>
+      </c>
+      <c r="E90" t="s">
         <v>190</v>
       </c>
-      <c r="B90" t="s">
-        <v>73</v>
-      </c>
-      <c r="C90" t="s">
-        <v>102</v>
-      </c>
-      <c r="E90" t="s">
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="B91" t="s">
+        <v>73</v>
+      </c>
+      <c r="C91" t="s">
+        <v>101</v>
+      </c>
+      <c r="E91" t="s">
         <v>192</v>
       </c>
-      <c r="B91" t="s">
-        <v>73</v>
-      </c>
-      <c r="C91" t="s">
-        <v>102</v>
-      </c>
-      <c r="E91" t="s">
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>194</v>
-      </c>
       <c r="B92" t="s">
         <v>73</v>
       </c>
       <c r="C92" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E92" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -2765,253 +2765,253 @@
         <v>73</v>
       </c>
       <c r="C93" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E93" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="B94" t="s">
+        <v>73</v>
+      </c>
+      <c r="C94" t="s">
+        <v>101</v>
+      </c>
+      <c r="E94" t="s">
         <v>196</v>
       </c>
-      <c r="B94" t="s">
-        <v>73</v>
-      </c>
-      <c r="C94" t="s">
-        <v>102</v>
-      </c>
-      <c r="E94" t="s">
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="B95" t="s">
+        <v>73</v>
+      </c>
+      <c r="C95" t="s">
+        <v>101</v>
+      </c>
+      <c r="E95" t="s">
         <v>198</v>
       </c>
-      <c r="B95" t="s">
-        <v>73</v>
-      </c>
-      <c r="C95" t="s">
-        <v>102</v>
-      </c>
-      <c r="E95" t="s">
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="B96" t="s">
+        <v>73</v>
+      </c>
+      <c r="C96" t="s">
+        <v>101</v>
+      </c>
+      <c r="E96" t="s">
         <v>200</v>
       </c>
-      <c r="B96" t="s">
-        <v>73</v>
-      </c>
-      <c r="C96" t="s">
-        <v>102</v>
-      </c>
-      <c r="E96" t="s">
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="B97" t="s">
+        <v>73</v>
+      </c>
+      <c r="C97" t="s">
+        <v>101</v>
+      </c>
+      <c r="E97" t="s">
         <v>202</v>
       </c>
-      <c r="B97" t="s">
-        <v>73</v>
-      </c>
-      <c r="C97" t="s">
-        <v>102</v>
-      </c>
-      <c r="E97" t="s">
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="B98" t="s">
+        <v>73</v>
+      </c>
+      <c r="C98" t="s">
+        <v>101</v>
+      </c>
+      <c r="E98" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
         <v>204</v>
       </c>
-      <c r="B98" t="s">
-        <v>73</v>
-      </c>
-      <c r="C98" t="s">
-        <v>102</v>
-      </c>
-      <c r="E98" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="B99" t="s">
+        <v>73</v>
+      </c>
+      <c r="C99" t="s">
+        <v>101</v>
+      </c>
+      <c r="E99" t="s">
         <v>205</v>
       </c>
-      <c r="B99" t="s">
-        <v>73</v>
-      </c>
-      <c r="C99" t="s">
-        <v>102</v>
-      </c>
-      <c r="E99" t="s">
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="B100" t="s">
+        <v>73</v>
+      </c>
+      <c r="C100" t="s">
+        <v>115</v>
+      </c>
+      <c r="E100" t="s">
         <v>207</v>
       </c>
-      <c r="B100" t="s">
-        <v>73</v>
-      </c>
-      <c r="C100" t="s">
-        <v>116</v>
-      </c>
-      <c r="E100" t="s">
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="B101" t="s">
+        <v>73</v>
+      </c>
+      <c r="C101" t="s">
+        <v>115</v>
+      </c>
+      <c r="E101" t="s">
         <v>209</v>
       </c>
-      <c r="B101" t="s">
-        <v>73</v>
-      </c>
-      <c r="C101" t="s">
-        <v>116</v>
-      </c>
-      <c r="E101" t="s">
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="B102" t="s">
+        <v>73</v>
+      </c>
+      <c r="C102" t="s">
+        <v>115</v>
+      </c>
+      <c r="E102" t="s">
         <v>211</v>
       </c>
-      <c r="B102" t="s">
-        <v>73</v>
-      </c>
-      <c r="C102" t="s">
-        <v>116</v>
-      </c>
-      <c r="E102" t="s">
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="B103" t="s">
+        <v>73</v>
+      </c>
+      <c r="C103" t="s">
+        <v>115</v>
+      </c>
+      <c r="E103" t="s">
         <v>213</v>
       </c>
-      <c r="B103" t="s">
-        <v>73</v>
-      </c>
-      <c r="C103" t="s">
-        <v>116</v>
-      </c>
-      <c r="E103" t="s">
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>215</v>
-      </c>
       <c r="B104" t="s">
         <v>73</v>
       </c>
       <c r="C104" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B105" t="s">
         <v>73</v>
       </c>
       <c r="C105" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="B106" t="s">
+        <v>73</v>
+      </c>
+      <c r="C106" t="s">
+        <v>115</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E106" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>218</v>
       </c>
-      <c r="B106" t="s">
-        <v>73</v>
-      </c>
-      <c r="C106" t="s">
-        <v>116</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E106" t="s">
+      <c r="B107" t="s">
+        <v>73</v>
+      </c>
+      <c r="C107" t="s">
+        <v>115</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E107" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>219</v>
       </c>
-      <c r="B107" t="s">
-        <v>73</v>
-      </c>
-      <c r="C107" t="s">
-        <v>116</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E107" t="s">
+      <c r="B108" t="s">
+        <v>73</v>
+      </c>
+      <c r="C108" t="s">
+        <v>115</v>
+      </c>
+      <c r="D108" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="E108" t="s">
         <v>220</v>
       </c>
-      <c r="B108" t="s">
-        <v>73</v>
-      </c>
-      <c r="C108" t="s">
-        <v>116</v>
-      </c>
-      <c r="D108" t="s">
-        <v>182</v>
-      </c>
-      <c r="E108" t="s">
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="B109" t="s">
+        <v>73</v>
+      </c>
+      <c r="C109" t="s">
+        <v>115</v>
+      </c>
+      <c r="D109" t="s">
+        <v>183</v>
+      </c>
+      <c r="E109" t="s">
         <v>222</v>
       </c>
-      <c r="B109" t="s">
-        <v>73</v>
-      </c>
-      <c r="C109" t="s">
-        <v>116</v>
-      </c>
-      <c r="D109" t="s">
-        <v>184</v>
-      </c>
-      <c r="E109" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B110" t="s">
         <v>74</v>
@@ -3020,12 +3020,12 @@
         <v>73</v>
       </c>
       <c r="E110" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B111" t="s">
         <v>74</v>
@@ -3034,12 +3034,12 @@
         <v>73</v>
       </c>
       <c r="E111" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B112" t="s">
         <v>74</v>
@@ -3048,12 +3048,12 @@
         <v>73</v>
       </c>
       <c r="E112" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B113" t="s">
         <v>74</v>
@@ -3062,12 +3062,12 @@
         <v>73</v>
       </c>
       <c r="E113" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>94</v>
+        <v>286</v>
       </c>
       <c r="B114" t="s">
         <v>74</v>
@@ -3076,13 +3076,13 @@
         <v>73</v>
       </c>
       <c r="D114" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E114" t="s">
         <v>147</v>
       </c>
-      <c r="E114" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>54</v>
       </c>
@@ -3093,15 +3093,15 @@
         <v>73</v>
       </c>
       <c r="D115" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E115" t="s">
         <v>149</v>
       </c>
-      <c r="E115" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B116" t="s">
         <v>74</v>
@@ -3110,12 +3110,12 @@
         <v>73</v>
       </c>
       <c r="E116" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B117" t="s">
         <v>74</v>
@@ -3124,97 +3124,97 @@
         <v>73</v>
       </c>
       <c r="E117" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B118" t="s">
         <v>74</v>
       </c>
       <c r="C118" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D118" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E118" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B119" t="s">
         <v>74</v>
       </c>
       <c r="C119" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D119" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E119" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B120" t="s">
         <v>74</v>
       </c>
       <c r="C120" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D120" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E120" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
+        <v>228</v>
+      </c>
+      <c r="B121" t="s">
+        <v>73</v>
+      </c>
+      <c r="C121" t="s">
+        <v>73</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B121" t="s">
-        <v>73</v>
-      </c>
-      <c r="C121" t="s">
-        <v>73</v>
-      </c>
-      <c r="D121" s="1" t="s">
+      <c r="E121" t="s">
         <v>230</v>
       </c>
-      <c r="E121" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B122" t="s">
         <v>74</v>
       </c>
       <c r="C122" t="s">
+        <v>231</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="E122" t="s">
         <v>233</v>
       </c>
-      <c r="E122" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B123" t="s">
         <v>74</v>
@@ -3223,58 +3223,58 @@
         <v>73</v>
       </c>
       <c r="D123" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E123" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="150" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="150" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="151" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="152" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="153" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="154" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="155" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="156" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="157" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="158" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="159" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="160" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="161" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="162" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="163" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="164" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="165" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="166" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="167" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="168" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="169" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="170" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="171" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="172" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="173" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="174" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="175" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="176" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="177" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="178" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="179" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="180" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="181" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="182" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="183" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="184" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="185" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="186" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="187" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="188" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="189" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="190" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="191" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="192" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="193" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="194" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="195" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D195">
     <sortCondition ref="A8:A195"/>

</xml_diff>